<commit_message>
added a new page (modificare discipline), updated dashboard, updated views
</commit_message>
<xml_diff>
--- a/media/Buget/Buget.xlsx
+++ b/media/Buget/Buget.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\40729\Desktop\Licenta\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F69F7513-2092-4FE3-A483-4B8859A8D0C8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8055B24A-8443-4E09-9BE7-E585052C6D76}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="62">
   <si>
     <t>Nume tema</t>
   </si>
@@ -118,13 +118,106 @@
   </si>
   <si>
     <t>Tema 30</t>
+  </si>
+  <si>
+    <t>Descriere</t>
+  </si>
+  <si>
+    <t>descriere 1</t>
+  </si>
+  <si>
+    <t>descriere 2</t>
+  </si>
+  <si>
+    <t>descriere 3</t>
+  </si>
+  <si>
+    <t>descriere 4</t>
+  </si>
+  <si>
+    <t>descriere 5</t>
+  </si>
+  <si>
+    <t>descriere 6</t>
+  </si>
+  <si>
+    <t>descriere 7</t>
+  </si>
+  <si>
+    <t>descriere 8</t>
+  </si>
+  <si>
+    <t>descriere 9</t>
+  </si>
+  <si>
+    <t>descriere 10</t>
+  </si>
+  <si>
+    <t>descriere 11</t>
+  </si>
+  <si>
+    <t>descriere 12</t>
+  </si>
+  <si>
+    <t>descriere 13</t>
+  </si>
+  <si>
+    <t>descriere 14</t>
+  </si>
+  <si>
+    <t>descriere 15</t>
+  </si>
+  <si>
+    <t>descriere 16</t>
+  </si>
+  <si>
+    <t>descriere 17</t>
+  </si>
+  <si>
+    <t>descriere 18</t>
+  </si>
+  <si>
+    <t>descriere 19</t>
+  </si>
+  <si>
+    <t>descriere 20</t>
+  </si>
+  <si>
+    <t>descriere 21</t>
+  </si>
+  <si>
+    <t>descriere 22</t>
+  </si>
+  <si>
+    <t>descriere 23</t>
+  </si>
+  <si>
+    <t>descriere 24</t>
+  </si>
+  <si>
+    <t>descriere 25</t>
+  </si>
+  <si>
+    <t>descriere 26</t>
+  </si>
+  <si>
+    <t>descriere 27</t>
+  </si>
+  <si>
+    <t>descriere 28</t>
+  </si>
+  <si>
+    <t>descriere 29</t>
+  </si>
+  <si>
+    <t>descriere 30</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -160,6 +253,15 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="238"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -181,11 +283,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -466,174 +569,267 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:A39"/>
+  <dimension ref="A1:B39"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="C23" sqref="C23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="22.88671875" style="2" customWidth="1"/>
-    <col min="2" max="2" width="8.88671875" customWidth="1"/>
+    <col min="2" max="2" width="11.5546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="2" spans="1:1" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="B1" s="4" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="3" spans="1:1" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="B2" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A3" s="3" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="4" spans="1:1" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="B3" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A4" s="3" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="5" spans="1:1" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="B4" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A5" s="3" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="6" spans="1:1" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="B5" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A6" s="3" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="7" spans="1:1" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="B6" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A7" s="3" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="8" spans="1:1" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="B7" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A8" s="3" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="9" spans="1:1" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="B8" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A9" s="3" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="10" spans="1:1" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="B9" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A10" s="3" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="11" spans="1:1" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="B10" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A11" s="3" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="12" spans="1:1" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="B11" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A12" s="3" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="13" spans="1:1" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="B12" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A13" s="3" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="14" spans="1:1" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="B13" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A14" s="3" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="15" spans="1:1" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="B14" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A15" s="3" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="16" spans="1:1" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="B15" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A16" s="3" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="17" spans="1:1" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="B16" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A17" s="3" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="18" spans="1:1" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="B17" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A18" s="3" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="19" spans="1:1" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="B18" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A19" s="3" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="20" spans="1:1" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="B19" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A20" s="3" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="21" spans="1:1" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="B20" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A21" s="3" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="22" spans="1:1" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="B21" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A22" s="3" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="23" spans="1:1" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="B22" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A23" s="3" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="24" spans="1:1" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="B23" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A24" s="3" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="25" spans="1:1" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="B24" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A25" s="3" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="26" spans="1:1" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="B25" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A26" s="3" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="27" spans="1:1" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="B26" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A27" s="3" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="28" spans="1:1" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="B27" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A28" s="3" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="29" spans="1:1" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="B28" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A29" s="3" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="30" spans="1:1" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="B29" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A30" s="3" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="31" spans="1:1" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="B30" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A31" s="3" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="32" spans="1:1" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="B31" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A32" s="3"/>
     </row>
     <row r="33" spans="1:1" ht="15.6" x14ac:dyDescent="0.3">

</xml_diff>